<commit_message>
change the para in excel
</commit_message>
<xml_diff>
--- a/router para.xlsx
+++ b/router para.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23613"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="20" windowWidth="18820" windowHeight="12120"/>
+    <workbookView xWindow="1060" yWindow="220" windowWidth="18820" windowHeight="12120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,31 +21,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>internal/external</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>nt</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -63,39 +45,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>local-as</t>
-  </si>
-  <si>
-    <t>ttl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>multihop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>ool</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>family inet</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>unicast/multicast/any</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>B</t>
     </r>
@@ -110,58 +59,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>cluster</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ip address</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bfd-liveness-detection</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>multipath</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hold-time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>minimum-interval</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>multiplier</t>
-  </si>
-  <si>
-    <t>import</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>str</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>export</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>str</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>neighbor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ip address</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>peer</t>
+    <t>peer-as</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -169,7 +67,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -185,10 +83,6 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="仿宋"/>
     </font>
   </fonts>
   <fills count="2">
@@ -213,14 +107,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -520,7 +411,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -536,128 +427,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="B2" s="3" t="s">
-        <v>25</v>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="B14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="B15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add protocol and attributes
</commit_message>
<xml_diff>
--- a/router para.xlsx
+++ b/router para.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23613"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="220" windowWidth="18820" windowHeight="12120"/>
+    <workbookView xWindow="120" yWindow="20" windowWidth="18820" windowHeight="12120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>internal/external</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>nt</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -45,6 +63,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>local-as</t>
+  </si>
+  <si>
+    <t>ttl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multihop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ool</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>family inet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unicast/multicast/any</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t>B</t>
     </r>
@@ -59,7 +110,62 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>peer-as</t>
+    <t>cluster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ip address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bfd-liveness-detection</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multipath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hold-time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>minimum-interval</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiplier</t>
+  </si>
+  <si>
+    <t>import</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>str</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>export</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>str</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>neighbor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ip address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>peer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSDP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -67,7 +173,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -83,6 +189,10 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="仿宋"/>
     </font>
   </fonts>
   <fills count="2">
@@ -107,11 +217,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -411,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -427,21 +540,133 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="4" spans="1:3">
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Exclude the ServerData2 Folder
</commit_message>
<xml_diff>
--- a/router para.xlsx
+++ b/router para.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23613"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="20" windowWidth="18820" windowHeight="12120"/>
+    <workbookView xWindow="4040" yWindow="1720" windowWidth="18820" windowHeight="12120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>bool</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -166,6 +166,22 @@
   </si>
   <si>
     <t>MSDP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HHH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ffff</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -524,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -664,9 +680,35 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>26</v>
+      </c>
+      <c r="B17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="B18">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="B23" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>